<commit_message>
changed to swap test
</commit_message>
<xml_diff>
--- a/Quamtun Machine Learning/output.xlsx
+++ b/Quamtun Machine Learning/output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmang\Codes\Quantum Algorithm\QiskitTutorial\Quamtun Machine Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA7C130-F8CA-4677-9A7F-B2F7B4C869AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE84B51-20EF-48E5-A254-0F790E9BF18C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4035" yWindow="3690" windowWidth="21600" windowHeight="11385" xr2:uid="{83647939-952A-4E48-81D2-610227AD6A3E}"/>
+    <workbookView xWindow="6855" yWindow="2175" windowWidth="21600" windowHeight="11385" xr2:uid="{83647939-952A-4E48-81D2-610227AD6A3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,11 +43,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>|0&gt;</t>
+    <t>|1&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>|1&gt;</t>
+    <t>|01&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -181,55 +181,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>809924</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>162374</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="그림 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E56599B-5111-D7CE-2C00-869431B7F2D0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2095500" y="2600325"/>
-          <a:ext cx="2143424" cy="3219899"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -532,7 +483,7 @@
   <dimension ref="B1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -548,10 +499,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
@@ -562,15 +513,15 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>0.48299999999999998</v>
+        <v>0.46600000000000003</v>
       </c>
       <c r="E2">
         <f>1-D2</f>
-        <v>0.51700000000000002</v>
+        <v>0.53400000000000003</v>
       </c>
       <c r="F2">
-        <f>2*D2-1</f>
-        <v>-3.400000000000003E-2</v>
+        <f>3-4*D2</f>
+        <v>1.1359999999999999</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
@@ -588,8 +539,8 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F9" si="1">2*D3-1</f>
-        <v>-9.9999999999999978E-2</v>
+        <f t="shared" ref="F3:F9" si="1">3-4*D3</f>
+        <v>1.2</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
@@ -608,7 +559,7 @@
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>-8.7999999999999967E-2</v>
+        <v>1.1759999999999999</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
@@ -626,8 +577,8 @@
         <v>0.51800000000000002</v>
       </c>
       <c r="F5">
-        <f>2*D5-1</f>
-        <v>-3.6000000000000032E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.0720000000000001</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
@@ -646,7 +597,7 @@
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>8.8000000000000078E-2</v>
+        <v>0.82399999999999984</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
@@ -665,7 +616,7 @@
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>1.0000000000000009E-2</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
@@ -684,7 +635,7 @@
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>0.1120000000000001</v>
+        <v>0.7759999999999998</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
@@ -703,13 +654,12 @@
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>2.0000000000000018E-2</v>
+        <v>0.96</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>